<commit_message>
updated excel iteration 2
</commit_message>
<xml_diff>
--- a/iteration_2_template.xlsx
+++ b/iteration_2_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/munaiman/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\caleb\Documents\GitHub\group-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D469B063-837C-7343-8BDE-69295D3210CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08BC4E4C-E764-4082-94C5-D7FC74C10755}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41200" yWindow="3500" windowWidth="23260" windowHeight="12580" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4236" yWindow="0" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Your Team Name</t>
   </si>
@@ -48,13 +48,43 @@
   </si>
   <si>
     <t>Scrum Master</t>
+  </si>
+  <si>
+    <t>A + C</t>
+  </si>
+  <si>
+    <t>Display movies with select actor(s)</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Display movies made after 1990 </t>
+  </si>
+  <si>
+    <t>A + D</t>
+  </si>
+  <si>
+    <t>Find movies with select song(s)</t>
+  </si>
+  <si>
+    <t>Display movies of a select genre</t>
+  </si>
+  <si>
+    <t>Display movies with select actor, and select genre</t>
+  </si>
+  <si>
+    <t>A + B</t>
+  </si>
+  <si>
+    <t>A + B + C</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -188,6 +218,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF220011"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="33">
@@ -531,7 +567,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -540,6 +576,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -901,29 +940,29 @@
       <selection activeCell="A5" sqref="A5:A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="21" style="1" customWidth="1"/>
-    <col min="2" max="2" width="30.1640625" customWidth="1"/>
+    <col min="2" max="2" width="30.109375" customWidth="1"/>
     <col min="3" max="3" width="21.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -934,37 +973,37 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>7</v>
       </c>
@@ -985,16 +1024,16 @@
   <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="27.33203125" customWidth="1"/>
-    <col min="3" max="3" width="68.5" customWidth="1"/>
+    <col min="3" max="3" width="68.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>6</v>
       </c>
@@ -1005,127 +1044,157 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>

</xml_diff>